<commit_message>
nettoyé les fichiers d'entrée
</commit_message>
<xml_diff>
--- a/data_env_2.xlsx
+++ b/data_env_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="74">
   <si>
     <t>annee</t>
   </si>
@@ -581,7 +581,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,6 +1018,21 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="L8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1233,8 +1248,26 @@
       <c r="D12" s="3">
         <v>1989</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="F12" s="3">
         <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>21</v>
@@ -1457,6 +1490,21 @@
       <c r="F16" s="2">
         <v>0</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>56</v>
       </c>
@@ -1659,44 +1707,62 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>2021</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1900</v>
       </c>
       <c r="E20" s="1">
         <v>12</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="F20" s="1">
+        <v>66</v>
+      </c>
+      <c r="G20" s="1">
+        <v>13</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>45</v>
+      </c>
+      <c r="J20" s="1">
+        <v>52</v>
+      </c>
+      <c r="K20" s="1">
+        <v>12</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q20" s="2" t="s">
+      <c r="M20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20" s="1">
         <v>47</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2231,106 +2297,121 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+    <row r="30" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>2021</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="1">
         <v>1989</v>
       </c>
       <c r="E30" s="1">
         <v>27</v>
       </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="L30" s="3" t="s">
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>54</v>
+      </c>
+      <c r="H30" s="1">
+        <v>25</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q30" s="3" t="s">
+      <c r="M30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30" s="1">
         <v>8</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="S30" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+    <row r="31" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>2021</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="1">
         <v>1989</v>
       </c>
       <c r="E31" s="1">
         <v>18</v>
       </c>
-      <c r="F31" s="3">
-        <v>0</v>
-      </c>
-      <c r="G31" s="3">
-        <v>64</v>
-      </c>
-      <c r="H31" s="3">
-        <v>13</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>75</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>12</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R31" s="1">
         <v>8</v>
       </c>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" s="3">
-        <v>12</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R31" s="3">
-        <v>8</v>
-      </c>
-      <c r="S31" s="3" t="s">
+      <c r="S31" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>